<commit_message>
Final commit with lot of minor errors solved
</commit_message>
<xml_diff>
--- a/php_files/angular.xlsx
+++ b/php_files/angular.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D820F1DB-11D5-4563-9D5A-047F98A1443F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73E630A-342A-4274-BCD2-6C15ED87F0A8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,20 +20,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Jagannath Pidaparthy</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
     <t>Vishal Patil</t>
   </si>
   <si>
-    <t>Prretika Shetty</t>
-  </si>
-  <si>
     <t>Sagar Mishra</t>
   </si>
   <si>
@@ -53,6 +47,9 @@
   </si>
   <si>
     <t>Purva Shinde</t>
+  </si>
+  <si>
+    <t>Preetika Shetty</t>
   </si>
 </sst>
 </file>
@@ -370,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,114 +379,111 @@
     <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1</v>
+        <v>52501</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>52502</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>52503</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>52504</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>52505</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
       </c>
       <c r="C5">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>6</v>
+        <v>52506</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>95.3</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>7</v>
+        <v>52507</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>8</v>
+        <v>52508</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>9</v>
+        <v>52509</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9">
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>10</v>
+        <v>52510</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <v>80</v>

</xml_diff>